<commit_message>
Corrigiendo errores en la búsqueda y edición de mensajes
</commit_message>
<xml_diff>
--- a/ProyectoFinal/casos_de_prueba.xlsx
+++ b/ProyectoFinal/casos_de_prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\Formación\Programación\Python\Coderhouse\ProyectoFinal\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869E8EB6-DF61-4919-A3FC-302909F36C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB63F1A-C9D7-4A61-99B0-1F3A14B5AFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6A476396-927E-4521-B9BD-CCBC8F182E28}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="45">
   <si>
     <t>Prueba #</t>
   </si>
@@ -126,6 +126,51 @@
   </si>
   <si>
     <t>Agregar Avatar</t>
+  </si>
+  <si>
+    <t>Usuario logueado</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>Mensaje: Datos Incorrectos. Intente nuevamente.</t>
+  </si>
+  <si>
+    <t>Usuario deslogueado</t>
+  </si>
+  <si>
+    <t>Nuevo registro de usuario</t>
+  </si>
+  <si>
+    <t>Avatar agregado</t>
+  </si>
+  <si>
+    <t>Especie creada</t>
+  </si>
+  <si>
+    <t>Especie modificada</t>
+  </si>
+  <si>
+    <t>Detalle de la especie visualizado</t>
+  </si>
+  <si>
+    <t>Especie borrada</t>
+  </si>
+  <si>
+    <t>Especie encontrada</t>
+  </si>
+  <si>
+    <t>Mensaje: No se encontraron especies con ese código</t>
+  </si>
+  <si>
+    <t>Mensaje posteado</t>
+  </si>
+  <si>
+    <t>Mensaje editado</t>
+  </si>
+  <si>
+    <t>Mensaje borrado</t>
   </si>
 </sst>
 </file>
@@ -582,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F77D0127-AB13-4023-9A8A-A2F215DE3E3A}">
   <dimension ref="A2:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +636,7 @@
     <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="20.5703125" customWidth="1"/>
+    <col min="4" max="5" width="48.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -630,70 +675,100 @@
         <v>1</v>
       </c>
       <c r="B4" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -730,56 +805,80 @@
         <v>1</v>
       </c>
       <c r="B12" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2</v>
       </c>
       <c r="B13" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>3</v>
       </c>
       <c r="B14" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>4</v>
       </c>
       <c r="B15" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -816,56 +915,80 @@
         <v>1</v>
       </c>
       <c r="B19" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2</v>
       </c>
       <c r="B20" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>3</v>
       </c>
       <c r="B21" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>4</v>
       </c>
       <c r="B22" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
@@ -902,56 +1025,80 @@
         <v>1</v>
       </c>
       <c r="B26" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2</v>
       </c>
       <c r="B27" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>3</v>
       </c>
       <c r="B28" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>4</v>
       </c>
       <c r="B29" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
@@ -988,56 +1135,80 @@
         <v>1</v>
       </c>
       <c r="B33" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2</v>
       </c>
       <c r="B34" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="D34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>3</v>
       </c>
       <c r="B35" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="D35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>4</v>
       </c>
       <c r="B36" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="D36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
@@ -1074,70 +1245,100 @@
         <v>1</v>
       </c>
       <c r="B40" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
+      <c r="D40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2</v>
       </c>
       <c r="B41" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
+      <c r="D41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>3</v>
       </c>
       <c r="B42" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+      <c r="D42" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>4</v>
       </c>
       <c r="B43" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
+      <c r="D43" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>5</v>
       </c>
       <c r="B44" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="D44" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
@@ -1174,42 +1375,60 @@
         <v>1</v>
       </c>
       <c r="B48" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2</v>
       </c>
       <c r="B49" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
+      <c r="D49" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>3</v>
       </c>
       <c r="B50" s="3">
-        <v>44901</v>
+        <v>44902</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
+      <c r="D50" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>